<commit_message>
01/10/2023    Kevin Jackey    Completed Brand Revenue section
</commit_message>
<xml_diff>
--- a/Data Files/Test Data Driver.xlsx
+++ b/Data Files/Test Data Driver.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinJackey\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KevinJackey\Katalon Studio\BTT_Katalon_Portal_Automation.git (3)\Data Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B193D89A-D094-4B5B-96F8-D14C3A937BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA93D6EA-F097-4690-8300-BA6BFB3189D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-13965" yWindow="-16470" windowWidth="29040" windowHeight="15840" xr2:uid="{239D9ABD-4136-4C6F-8CEA-C3B045C3DDF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>action</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>validate</t>
+  </si>
+  <si>
+    <t>Object Repository/Filters/Main Filter Window/Browsers and Devices/radio_IncludeBots</t>
+  </si>
+  <si>
+    <t>Include bots</t>
   </si>
 </sst>
 </file>
@@ -498,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669FA6DA-ABB3-4A3C-BD6C-F84189C85B2B}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,7 +517,7 @@
     <col min="3" max="3" width="18.109375" customWidth="1"/>
     <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="85.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="106.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -628,10 +634,10 @@
         <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -639,10 +645,10 @@
         <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -650,10 +656,10 @@
         <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -661,10 +667,10 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -672,10 +678,10 @@
         <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -683,20 +689,31 @@
         <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
         <v>34</v>
       </c>
       <c r="F17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>